<commit_message>
Correct Supplementary Table 5
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_5.xlsx
+++ b/Figures_Tables/Supp_Table_5.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t xml:space="preserve">File name in Github</t>
   </si>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Registered COVID deaths</t>
   </si>
   <si>
-    <t xml:space="preserve">0-17</t>
+    <t xml:space="preserve">0-2,3-11,12-17</t>
   </si>
   <si>
     <t xml:space="preserve">2020-01-01 to 2022-05-06</t>
@@ -145,19 +145,28 @@
     <t xml:space="preserve">Supp Fig 1 &amp; 2</t>
   </si>
   <si>
-    <t xml:space="preserve">public_access_2023.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccination status (2 or more doses) January 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-2,3-11,12-17</t>
+    <t xml:space="preserve">vac1_2023.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population vaccined with 1 dose on January 18th 2023</t>
   </si>
   <si>
     <t xml:space="preserve">January 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Table 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vac2_2023.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population vaccined with 2 doses on January 18th 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vac3_2023.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population vaccined with 3 or more doses on January 18th 2023</t>
   </si>
 </sst>
 </file>
@@ -306,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -530,15 +539,55 @@
         <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Supplementary Table 5
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_5.xlsx
+++ b/Figures_Tables/Supp_Table_5.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">All</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig 2, Table 1, Table 2</t>
+    <t xml:space="preserve">Figure 2, Table 1, Table 2</t>
   </si>
   <si>
     <t xml:space="preserve">National Registry of People, Argentina (RENAPER)</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">2020-01-01 to 2022-05-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig 2</t>
+    <t xml:space="preserve">Figure 2</t>
   </si>
   <si>
     <t xml:space="preserve">Freedom of information request</t>
@@ -97,6 +97,18 @@
     <t xml:space="preserve">2022-01-24 to 2022-12-31</t>
   </si>
   <si>
+    <t xml:space="preserve">data.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered COVID cases and deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-01-01 to 2022-12-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">provincias.zip</t>
   </si>
   <si>
@@ -112,18 +124,6 @@
     <t xml:space="preserve">National Geographic Institute, Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">data.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registered COVID cases and deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020-01-01 to 2022-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fig 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">grouped_df.gz</t>
   </si>
   <si>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">2020-2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Fig 2, Tables 3 &amp; 4</t>
+    <t xml:space="preserve">Figure 2, Tables 3 &amp; 4</t>
   </si>
   <si>
     <t xml:space="preserve">grouped_df2.gz</t>
@@ -315,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,7 +459,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>27</v>
@@ -468,27 +468,27 @@
         <v>28</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -548,7 +548,7 @@
         <v>44</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -568,7 +568,7 @@
         <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -588,9 +588,10 @@
         <v>44</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Updated all figures to use the same vaccination database
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_5.xlsx
+++ b/Figures_Tables/Supp_Table_5.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t xml:space="preserve">File name in Github</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Data contained</t>
   </si>
   <si>
-    <t xml:space="preserve">Age group</t>
+    <t xml:space="preserve">Age groups</t>
   </si>
   <si>
     <t xml:space="preserve">Period</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">fall_1.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">Registered COVID deaths</t>
+    <t xml:space="preserve">Registered COVID deaths and their vaccination status</t>
   </si>
   <si>
     <t xml:space="preserve">0-2,3-11,12-17</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">2020-01-01 to 2022-05-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Figure 2</t>
+    <t xml:space="preserve">Figure 2, Tables 3 &amp; 4</t>
   </si>
   <si>
     <t xml:space="preserve">Freedom of information request</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">data.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">Registered COVID cases and deaths</t>
+    <t xml:space="preserve">Registered COVID cases, deaths and their vaccination status</t>
   </si>
   <si>
     <t xml:space="preserve">2020-01-01 to 2022-12-31</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">Geographic shape files</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">NA</t>
   </si>
   <si>
     <t xml:space="preserve">Supp Fig 2</t>
@@ -124,49 +124,16 @@
     <t xml:space="preserve">National Geographic Institute, Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">grouped_df.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pediatric Vaccination data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-11,12-17</t>
+    <t xml:space="preserve">vacnew.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pediatric Vaccination data – monthly</t>
   </si>
   <si>
     <t xml:space="preserve">2020-2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Figure 2, Tables 3 &amp; 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grouped_df2.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supp Fig 1 &amp; 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vac1_2023.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population vaccined with 1 dose on January 18th 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vac2_2023.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population vaccined with 2 doses on January 18th 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vac3_2023.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population vaccined with 3 or more doses on January 18th 2023</t>
+    <t xml:space="preserve">Table 1, Figure 2, Supp Fig 1 and Supp Fig 2</t>
   </si>
 </sst>
 </file>
@@ -176,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -221,6 +188,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -265,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,10 +248,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,15 +256,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -318,16 +283,16 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.75"/>
   </cols>
   <sheetData>
@@ -347,250 +312,175 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="4" t="n">
         <v>2021</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Modify Supp Table 5
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_5.xlsx
+++ b/Figures_Tables/Supp_Table_5.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Figure 2, Tables 3 &amp; 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Freedom of information request</t>
+    <t xml:space="preserve">Freedom of information request, National Ministry of Health, Argentina</t>
   </si>
   <si>
     <t xml:space="preserve">fall_2.xlsx</t>
@@ -283,7 +283,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix Supp Table 5
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_5.xlsx
+++ b/Figures_Tables/Supp_Table_5.xlsx
@@ -273,16 +273,16 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="50.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.75"/>
   </cols>
   <sheetData>

</xml_diff>